<commit_message>
Finished initial coding of Q6 definitions.
</commit_message>
<xml_diff>
--- a/data/derived/public/analysis_Q6_coding.xlsx
+++ b/data/derived/public/analysis_Q6_coding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahbardin/Desktop/OR-Reproducibility-in-Geography-Survey/data/derived/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7D5146-AC35-7F44-BD8D-BBC656BB1A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E93DA5-300D-2046-99F0-00B0D244D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="458">
   <si>
     <t>ResponseId</t>
   </si>
@@ -1397,6 +1397,24 @@
   </si>
   <si>
     <t>come back to</t>
+  </si>
+  <si>
+    <t>Not a definition</t>
+  </si>
+  <si>
+    <t>not sure</t>
+  </si>
+  <si>
+    <t>unclear how to code</t>
+  </si>
+  <si>
+    <t>Unsure</t>
+  </si>
+  <si>
+    <t>not a definition</t>
+  </si>
+  <si>
+    <t>Unclear how to code</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1749,6 +1767,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1910,7 +1934,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1937,6 +1961,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2298,9 +2326,9 @@
   <dimension ref="A1:P219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
+      <selection pane="bottomLeft" activeCell="N167" sqref="N167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4891,7 +4919,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4923,7 +4951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4946,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4962,8 +4990,17 @@
       <c r="E115" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4979,8 +5016,17 @@
       <c r="E116" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4996,8 +5042,17 @@
       <c r="E117" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="F117">
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5013,8 +5068,14 @@
       <c r="E118" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="F118">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5030,8 +5091,20 @@
       <c r="E119" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="N119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5047,25 +5120,34 @@
       <c r="E120" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A121">
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="J120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" s="14" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A121" s="14">
         <v>120</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D121" t="s">
-        <v>19</v>
-      </c>
-      <c r="E121" s="1" t="s">
+      <c r="D121" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E121" s="15" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="P121" s="14" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5081,8 +5163,14 @@
       <c r="E122" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5098,8 +5186,11 @@
       <c r="E123" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="J123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5115,8 +5206,11 @@
       <c r="E124" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="F124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5132,8 +5226,17 @@
       <c r="E125" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5149,8 +5252,17 @@
       <c r="E126" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="F126">
+        <v>1</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5166,8 +5278,17 @@
       <c r="E127" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="F127">
+        <v>1</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5183,8 +5304,17 @@
       <c r="E128" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5200,8 +5330,17 @@
       <c r="E129" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5217,8 +5356,11 @@
       <c r="E130" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="J130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5234,8 +5376,14 @@
       <c r="E131" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5251,8 +5399,14 @@
       <c r="E132" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5268,8 +5422,14 @@
       <c r="E133" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5285,8 +5445,14 @@
       <c r="E134" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5302,8 +5468,14 @@
       <c r="E135" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="K135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5319,8 +5491,14 @@
       <c r="E136" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5340,7 +5518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5356,25 +5534,34 @@
       <c r="E138" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A139">
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A139" s="14">
         <v>138</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D139" t="s">
-        <v>6</v>
-      </c>
-      <c r="E139" s="1" t="s">
+      <c r="D139" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" s="15" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="P139" s="14" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5390,8 +5577,11 @@
       <c r="E140" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="N140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5411,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5427,8 +5617,14 @@
       <c r="E142" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5444,8 +5640,17 @@
       <c r="E143" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5461,8 +5666,14 @@
       <c r="E144" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5482,7 +5693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5502,24 +5713,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A147">
+    <row r="147" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" s="14">
         <v>146</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E147" s="1" t="s">
+      <c r="E147" s="15" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="O147" s="14">
+        <v>1</v>
+      </c>
+      <c r="P147" s="14" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5535,8 +5752,14 @@
       <c r="E148" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5552,8 +5775,14 @@
       <c r="E149" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" ht="204" x14ac:dyDescent="0.2">
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5569,8 +5798,23 @@
       <c r="E150" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="F150">
+        <v>1</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5586,8 +5830,17 @@
       <c r="E151" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="M151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5603,8 +5856,14 @@
       <c r="E152" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5620,8 +5879,20 @@
       <c r="E153" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="M153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5637,8 +5908,17 @@
       <c r="E154" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F154">
+        <v>1</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5658,24 +5938,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A156">
+    <row r="156" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A156" s="14">
         <v>155</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D156" t="s">
-        <v>6</v>
-      </c>
-      <c r="E156" s="1" t="s">
+      <c r="D156" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" s="15" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="P156" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5691,8 +5974,17 @@
       <c r="E157" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5708,8 +6000,14 @@
       <c r="E158" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="K158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5725,8 +6023,14 @@
       <c r="E159" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="K159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5742,22 +6046,34 @@
       <c r="E160" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161">
+      <c r="F160">
+        <v>1</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" s="14">
         <v>160</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D161" t="s">
-        <v>19</v>
-      </c>
-      <c r="E161" s="1" t="s">
+      <c r="D161" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E161" s="15" t="s">
         <v>315</v>
+      </c>
+      <c r="H161" s="14">
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -5776,6 +6092,12 @@
       <c r="E162" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="M162">
+        <v>1</v>
+      </c>
     </row>
     <row r="163" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -5793,6 +6115,12 @@
       <c r="E163" s="1" t="s">
         <v>319</v>
       </c>
+      <c r="F163">
+        <v>1</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -5810,6 +6138,15 @@
       <c r="E164" s="1" t="s">
         <v>321</v>
       </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <v>1</v>
+      </c>
     </row>
     <row r="165" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -5827,6 +6164,12 @@
       <c r="E165" s="1" t="s">
         <v>323</v>
       </c>
+      <c r="J165">
+        <v>1</v>
+      </c>
+      <c r="K165">
+        <v>1</v>
+      </c>
     </row>
     <row r="166" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -5844,6 +6187,15 @@
       <c r="E166" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="F166">
+        <v>1</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>1</v>
+      </c>
     </row>
     <row r="167" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A167">
@@ -5861,6 +6213,12 @@
       <c r="E167" s="1" t="s">
         <v>327</v>
       </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+      <c r="J167">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A168">
@@ -5878,6 +6236,9 @@
       <c r="E168" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
     </row>
     <row r="169" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
@@ -5915,6 +6276,18 @@
       <c r="E170" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="F170">
+        <v>1</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="N170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A171">
@@ -5932,6 +6305,12 @@
       <c r="E171" s="1" t="s">
         <v>334</v>
       </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="J171">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A172">
@@ -5949,6 +6328,9 @@
       <c r="E172" s="1" t="s">
         <v>336</v>
       </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
     </row>
     <row r="173" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A173">
@@ -5966,6 +6348,12 @@
       <c r="E173" s="1" t="s">
         <v>338</v>
       </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+      <c r="M173">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A174">
@@ -5983,6 +6371,18 @@
       <c r="E174" s="1" t="s">
         <v>340</v>
       </c>
+      <c r="I174">
+        <v>1</v>
+      </c>
+      <c r="K174">
+        <v>1</v>
+      </c>
+      <c r="M174">
+        <v>1</v>
+      </c>
+      <c r="N174">
+        <v>1</v>
+      </c>
     </row>
     <row r="175" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A175">
@@ -6000,6 +6400,15 @@
       <c r="E175" s="1" t="s">
         <v>342</v>
       </c>
+      <c r="H175">
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>1</v>
+      </c>
+      <c r="K175">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A176">
@@ -6017,25 +6426,31 @@
       <c r="E176" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A177">
+      <c r="J176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A177" s="14">
         <v>176</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D177" t="s">
-        <v>19</v>
-      </c>
-      <c r="E177" s="1" t="s">
+      <c r="D177" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E177" s="15" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P177" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6051,8 +6466,17 @@
       <c r="E178" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="F178">
+        <v>1</v>
+      </c>
+      <c r="H178">
+        <v>1</v>
+      </c>
+      <c r="J178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6068,25 +6492,34 @@
       <c r="E179" s="1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A180">
+      <c r="H179">
+        <v>1</v>
+      </c>
+      <c r="K179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A180" s="14">
         <v>179</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D180" t="s">
-        <v>6</v>
-      </c>
-      <c r="E180" s="1" t="s">
+      <c r="D180" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E180" s="15" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P180" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6102,8 +6535,11 @@
       <c r="E181" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="J181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6119,8 +6555,11 @@
       <c r="E182" s="1" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="H182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6136,8 +6575,17 @@
       <c r="E183" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="F183">
+        <v>1</v>
+      </c>
+      <c r="H183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6153,8 +6601,14 @@
       <c r="E184" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="H184">
+        <v>1</v>
+      </c>
+      <c r="M184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6170,8 +6624,11 @@
       <c r="E185" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="186" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6191,7 +6648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6207,25 +6664,34 @@
       <c r="E187" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="188" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A188">
+      <c r="F187">
+        <v>1</v>
+      </c>
+      <c r="J187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A188" s="14">
         <v>187</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D188" t="s">
-        <v>19</v>
-      </c>
-      <c r="E188" s="1" t="s">
+      <c r="D188" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E188" s="15" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="O188" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6241,8 +6707,14 @@
       <c r="E189" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="190" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="H189">
+        <v>1</v>
+      </c>
+      <c r="M189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6258,25 +6730,31 @@
       <c r="E190" s="1" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A191">
+      <c r="J190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A191" s="14">
         <v>190</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D191" t="s">
-        <v>19</v>
-      </c>
-      <c r="E191" s="1" t="s">
+      <c r="D191" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E191" s="15" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="P191" s="14" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6296,7 +6774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6312,8 +6790,14 @@
       <c r="E193" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="H193">
+        <v>1</v>
+      </c>
+      <c r="M193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6329,25 +6813,37 @@
       <c r="E194" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195">
+      <c r="H194">
+        <v>1</v>
+      </c>
+      <c r="K194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A195" s="14">
         <v>194</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D195" t="s">
-        <v>6</v>
-      </c>
-      <c r="E195" s="1" t="s">
+      <c r="D195" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E195" s="15" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="H195" s="14">
+        <v>1</v>
+      </c>
+      <c r="M195" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6363,8 +6859,14 @@
       <c r="E196" s="1" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F196">
+        <v>1</v>
+      </c>
+      <c r="J196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6380,8 +6882,14 @@
       <c r="E197" s="1" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="H197">
+        <v>1</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6397,8 +6905,17 @@
       <c r="E198" s="1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="H198">
+        <v>1</v>
+      </c>
+      <c r="M198">
+        <v>1</v>
+      </c>
+      <c r="N198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6414,25 +6931,40 @@
       <c r="E199" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A200">
+      <c r="H199">
+        <v>1</v>
+      </c>
+      <c r="J199">
+        <v>1</v>
+      </c>
+      <c r="K199">
+        <v>1</v>
+      </c>
+      <c r="M199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A200" s="14">
         <v>199</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E200" s="15" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F200" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6448,8 +6980,17 @@
       <c r="E201" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F201">
+        <v>1</v>
+      </c>
+      <c r="H201">
+        <v>1</v>
+      </c>
+      <c r="J201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6465,8 +7006,17 @@
       <c r="E202" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="I202">
+        <v>1</v>
+      </c>
+      <c r="J202">
+        <v>1</v>
+      </c>
+      <c r="L202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6482,8 +7032,14 @@
       <c r="E203" s="1" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="H203">
+        <v>1</v>
+      </c>
+      <c r="J203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6499,8 +7055,17 @@
       <c r="E204" s="1" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="H204">
+        <v>1</v>
+      </c>
+      <c r="J204">
+        <v>1</v>
+      </c>
+      <c r="K204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6516,25 +7081,31 @@
       <c r="E205" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206">
+      <c r="J205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A206" s="14">
         <v>205</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D206" t="s">
-        <v>19</v>
-      </c>
-      <c r="E206" s="1" t="s">
+      <c r="D206" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E206" s="15" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="J206" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6550,8 +7121,14 @@
       <c r="E207" s="1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="H207">
+        <v>1</v>
+      </c>
+      <c r="J207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6567,8 +7144,14 @@
       <c r="E208" s="1" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="209" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="F208">
+        <v>1</v>
+      </c>
+      <c r="H208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6584,8 +7167,14 @@
       <c r="E209" s="1" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="210" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="F209">
+        <v>1</v>
+      </c>
+      <c r="H209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6601,8 +7190,17 @@
       <c r="E210" s="1" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="211" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="F210">
+        <v>1</v>
+      </c>
+      <c r="H210">
+        <v>1</v>
+      </c>
+      <c r="M210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6618,25 +7216,37 @@
       <c r="E211" s="1" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="212" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A212">
+      <c r="F211">
+        <v>1</v>
+      </c>
+      <c r="H211">
+        <v>1</v>
+      </c>
+      <c r="J211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A212" s="14">
         <v>211</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D212" t="s">
-        <v>19</v>
-      </c>
-      <c r="E212" s="1" t="s">
+      <c r="D212" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E212" s="15" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="213" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="P212" s="14" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6652,8 +7262,17 @@
       <c r="E213" s="1" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="214" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H213">
+        <v>1</v>
+      </c>
+      <c r="K213">
+        <v>1</v>
+      </c>
+      <c r="M213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6669,8 +7288,11 @@
       <c r="E214" s="1" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="215" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="J214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6686,25 +7308,31 @@
       <c r="E215" s="1" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="216" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A216">
+      <c r="H215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A216" s="14">
         <v>215</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E216" s="1" t="s">
+      <c r="E216" s="15" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="217" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P216" s="14" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6720,8 +7348,17 @@
       <c r="E217" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="218" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F217">
+        <v>1</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+      <c r="K217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6741,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6756,6 +7393,15 @@
       </c>
       <c r="E219" s="1" t="s">
         <v>427</v>
+      </c>
+      <c r="F219">
+        <v>1</v>
+      </c>
+      <c r="H219">
+        <v>1</v>
+      </c>
+      <c r="K219">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>